<commit_message>
added wait between cart & checkout
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC28_Verify_PlaceOrder_SelfService_SingleUser.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC28_Verify_PlaceOrder_SelfService_SingleUser.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_Muitisite\Input_files\Actual_testcases\Kaman\ECTEST\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94345979-0D5E-484F-9E42-E41BF7C37F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F818CC-3F21-4F58-89D5-E58B1FADF92A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="112">
   <si>
     <t>TestCase</t>
   </si>
@@ -791,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1062,51 +1062,51 @@
     <row r="22" spans="1:5">
       <c r="A22" s="3"/>
       <c r="B22" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>99</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="5"/>
       <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="3"/>
       <c r="B23" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>99</v>
+      </c>
       <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="3"/>
       <c r="B24" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>99</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="3"/>
       <c r="B25" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="3"/>
       <c r="B26" s="5" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -1115,44 +1115,44 @@
     <row r="27" spans="1:5">
       <c r="A27" s="3"/>
       <c r="B27" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>99</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3"/>
       <c r="B28" s="5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>83</v>
-      </c>
+      <c r="E28" s="3"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3"/>
       <c r="B29" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3"/>
       <c r="B30" s="5" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -1161,25 +1161,21 @@
     <row r="31" spans="1:5">
       <c r="A31" s="3"/>
       <c r="B31" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>99</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
       <c r="E31" s="3"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3"/>
       <c r="B32" s="5" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D32" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>99</v>
       </c>
       <c r="E32" s="3"/>
@@ -1187,7 +1183,7 @@
     <row r="33" spans="1:5">
       <c r="A33" s="3"/>
       <c r="B33" s="5" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>84</v>
@@ -1195,27 +1191,27 @@
       <c r="D33" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>84</v>
-      </c>
+      <c r="E33" s="3"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3"/>
       <c r="B34" s="5" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E34" s="3"/>
+      <c r="E34" s="3" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3"/>
       <c r="B35" s="5" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>85</v>
@@ -1223,27 +1219,27 @@
       <c r="D35" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E35" s="3" t="s">
-        <v>85</v>
-      </c>
+      <c r="E35" s="3"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3"/>
       <c r="B36" s="5" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E36" s="3"/>
+      <c r="E36" s="3" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3"/>
       <c r="B37" s="5" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>86</v>
@@ -1251,27 +1247,27 @@
       <c r="D37" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E37" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="E37" s="3"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3"/>
       <c r="B38" s="5" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E38" s="3"/>
+      <c r="E38" s="3" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3"/>
       <c r="B39" s="5" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>87</v>
@@ -1279,27 +1275,27 @@
       <c r="D39" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E39" s="3" t="s">
-        <v>87</v>
-      </c>
+      <c r="E39" s="3"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3"/>
       <c r="B40" s="5" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E40" s="3"/>
+      <c r="E40" s="3" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="3"/>
       <c r="B41" s="5" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>88</v>
@@ -1307,23 +1303,27 @@
       <c r="D41" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E41" s="3" t="s">
-        <v>88</v>
-      </c>
+      <c r="E41" s="3"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="3"/>
       <c r="B42" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
+        <v>70</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3"/>
       <c r="B43" s="5" t="s">
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -1332,23 +1332,23 @@
     <row r="44" spans="1:5">
       <c r="A44" s="3"/>
       <c r="B44" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>99</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
       <c r="E44" s="3"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3"/>
       <c r="B45" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>99</v>
+      </c>
       <c r="E45" s="3"/>
     </row>
     <row r="46" spans="1:5">
@@ -1363,17 +1363,11 @@
     <row r="47" spans="1:5">
       <c r="A47" s="3"/>
       <c r="B47" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>91</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C47" s="3"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="3"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3"/>
@@ -1381,43 +1375,43 @@
         <v>9</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>99</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3"/>
       <c r="B49" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C49" s="3"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3"/>
       <c r="B50" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>92</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C50" s="3"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="3"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="3"/>
       <c r="B51" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>92</v>
@@ -1425,36 +1419,36 @@
       <c r="D51" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E51" s="3"/>
+      <c r="E51" s="3" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="3"/>
       <c r="B52" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C52" s="3"/>
-      <c r="D52" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>99</v>
+      </c>
       <c r="E52" s="3"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3"/>
-      <c r="B53" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>111</v>
-      </c>
+      <c r="B53" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C53" s="3"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="3"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="3"/>
-      <c r="B54" s="3" t="s">
-        <v>96</v>
+      <c r="B54" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>97</v>
@@ -1463,6 +1457,21 @@
         <v>99</v>
       </c>
       <c r="E54" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E55" s="5" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1962,6 +1971,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006B9247FD3B8DCE459B42E632A3609B44" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3308c0b5f2a874e4881ed9e3e8048963">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a153bf7-9590-4a62-91b6-0515f1c483dc" xmlns:ns3="fd27ab66-8f5a-4733-8e24-c3cb82244a05" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afaafca1b8c32e4865f6f60996200392" ns2:_="" ns3:_="">
     <xsd:import namespace="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
@@ -2158,36 +2182,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F47607-34AD-43FE-B910-18186D4DE9CC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
-    <ds:schemaRef ds:uri="fd27ab66-8f5a-4733-8e24-c3cb82244a05"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2210,9 +2208,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F47607-34AD-43FE-B910-18186D4DE9CC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
+    <ds:schemaRef ds:uri="fd27ab66-8f5a-4733-8e24-c3cb82244a05"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>